<commit_message>
add coords excel input
</commit_message>
<xml_diff>
--- a/paneldata_new_withSeal.xlsx
+++ b/paneldata_new_withSeal.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CADInput" sheetId="1" r:id="rId1"/>
-    <sheet name="Normal" sheetId="2" r:id="rId2"/>
-    <sheet name="RFQ" sheetId="3" r:id="rId3"/>
+    <sheet name="SealData" sheetId="4" r:id="rId2"/>
+    <sheet name="Normal" sheetId="2" r:id="rId3"/>
+    <sheet name="RFQ" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="99">
   <si>
     <t>实测数据</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -350,6 +351,66 @@
   </si>
   <si>
     <t>Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glass方向上AA尺寸</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>引线偏移距离</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>传统屏幕四边Seal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>异形屏幕Seal封边</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>字号大小</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字体颜色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>偏移尺寸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>坐标总数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>距AA中心偏移位置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>距离</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -361,7 +422,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +454,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
       <family val="2"/>
@@ -564,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -599,6 +675,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -611,46 +693,64 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1042,23 +1142,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:T22"/>
+  <dimension ref="B1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="14.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.15">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B2" s="18" t="s">
         <v>29</v>
       </c>
@@ -1085,14 +1185,8 @@
       <c r="M2" s="19"/>
       <c r="N2" s="19"/>
       <c r="O2" s="20"/>
-      <c r="Q2" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-    </row>
-    <row r="3" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B3" s="21" t="s">
         <v>2</v>
       </c>
@@ -1132,22 +1226,9 @@
         <f>N3/1000</f>
         <v>428.04</v>
       </c>
-      <c r="Q3" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="S3" s="29">
-        <v>500</v>
-      </c>
-      <c r="T3" s="2">
-        <f>S3/1000</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B4" s="23"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B4" s="22"/>
       <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1157,7 +1238,7 @@
       <c r="E4" s="5">
         <v>120.96</v>
       </c>
-      <c r="G4" s="23"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1168,7 +1249,7 @@
         <f>I4/1000</f>
         <v>127.01</v>
       </c>
-      <c r="L4" s="23"/>
+      <c r="L4" s="22"/>
       <c r="M4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1178,19 +1259,8 @@
       <c r="O4" s="5">
         <v>535.19000000000005</v>
       </c>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="S4" s="29">
-        <v>600</v>
-      </c>
-      <c r="T4" s="2">
-        <f t="shared" ref="T4:T6" si="0">S4/1000</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B5" s="21" t="s">
         <v>30</v>
       </c>
@@ -1201,7 +1271,7 @@
         <v>850</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E9" si="1">D5/1000</f>
+        <f t="shared" ref="E5:E9" si="0">D5/1000</f>
         <v>0.85</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -1228,20 +1298,9 @@
       <c r="O5" s="5">
         <v>2</v>
       </c>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="S5" s="29">
-        <v>700</v>
-      </c>
-      <c r="T5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B6" s="23"/>
       <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
@@ -1249,7 +1308,7 @@
         <v>2300</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="G6" s="9" t="s">
@@ -1276,20 +1335,9 @@
       <c r="O6" s="5">
         <v>3</v>
       </c>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="S6" s="29">
-        <v>8000</v>
-      </c>
-      <c r="T6" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B7" s="23"/>
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1297,7 +1345,7 @@
         <v>800</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="G7" s="21" t="s">
@@ -1310,7 +1358,7 @@
         <v>14062</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" ref="J7:J12" si="2">I7/1000</f>
+        <f t="shared" ref="J7:J12" si="1">I7/1000</f>
         <v>14.061999999999999</v>
       </c>
       <c r="L7" s="21" t="s">
@@ -1323,12 +1371,12 @@
         <v>11870</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" ref="O7:O12" si="3">N7/1000</f>
+        <f t="shared" ref="O7:O12" si="2">N7/1000</f>
         <v>11.87</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B8" s="22"/>
       <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1336,10 +1384,10 @@
         <v>800</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G8" s="22"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="9" t="s">
         <v>6</v>
       </c>
@@ -1347,10 +1395,10 @@
         <v>13088</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13.087999999999999</v>
       </c>
-      <c r="L8" s="22"/>
+      <c r="L8" s="23"/>
       <c r="M8" s="9" t="s">
         <v>6</v>
       </c>
@@ -1358,11 +1406,11 @@
         <v>12500</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
         <v>31</v>
       </c>
@@ -1373,10 +1421,10 @@
         <v>2900</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.9</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1384,10 +1432,10 @@
         <v>5100</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="L9" s="22"/>
+      <c r="L9" s="23"/>
       <c r="M9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1395,11 +1443,11 @@
         <v>7940</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.94</v>
       </c>
     </row>
-    <row r="10" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B10" s="8" t="s">
         <v>37</v>
       </c>
@@ -1412,7 +1460,7 @@
       <c r="E10" s="7">
         <v>0</v>
       </c>
-      <c r="G10" s="23"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="9" t="s">
         <v>8</v>
       </c>
@@ -1420,10 +1468,10 @@
         <v>5100</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="L10" s="23"/>
+      <c r="L10" s="22"/>
       <c r="M10" s="9" t="s">
         <v>8</v>
       </c>
@@ -1431,20 +1479,20 @@
         <v>7940</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.94</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>34</v>
+      <c r="E11" s="37" t="s">
+        <v>94</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>15</v>
@@ -1456,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L11" s="21" t="s">
@@ -1469,12 +1517,12 @@
         <v>5250</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.25</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="G12" s="23"/>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="G12" s="22"/>
       <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
@@ -1482,10 +1530,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="23"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="22"/>
       <c r="M12" s="9" t="s">
         <v>17</v>
       </c>
@@ -1493,11 +1541,11 @@
         <v>0</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.15">
       <c r="G13" s="9" t="s">
         <v>18</v>
       </c>
@@ -1511,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.15">
       <c r="G14" s="10" t="s">
         <v>74</v>
       </c>
@@ -1525,16 +1573,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B21" s="3">
         <f>E3+E7+E8+E10</f>
         <v>69.64</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16" t="str">
+      <c r="D21" s="15"/>
+      <c r="E21" s="24" t="str">
         <f>IF(AND(J3=B21,J4=B22),"OK","BAD")</f>
         <v>OK</v>
       </c>
@@ -1542,11 +1590,11 @@
         <f>IF((J13=0),J3*J6+(J6-1)*J12+J9+J10,J4*J6+(J6-1)*J12+J9+J10)</f>
         <v>428.04000000000008</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="16" t="str">
+      <c r="I21" s="15"/>
+      <c r="J21" s="24" t="str">
         <f>IF(AND(O3=G21,O4=G22),"OK","BAD")</f>
         <v>OK</v>
       </c>
@@ -1554,42 +1602,44 @@
         <f>O3*O6+(O6-1)*O12++O9+O10</f>
         <v>1300.0000000000002</v>
       </c>
-      <c r="M21" s="12" t="s">
+      <c r="M21" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="13"/>
-      <c r="O21" s="16" t="str">
+      <c r="N21" s="15"/>
+      <c r="O21" s="24" t="str">
         <f>IF(AND(1300=L21,1100=L22),"OK","BAD")</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B22" s="3">
         <f>E4+E5+E6+E9</f>
         <v>127.00999999999999</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="17"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="25"/>
       <c r="G22" s="1">
         <f>IF((J13=0),J4*J5+(J5-1)*J11+J7+J8,J3*J5+(J5-1)*J11+J7+J8)</f>
         <v>535.18999999999994</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="25"/>
       <c r="L22" s="1">
         <f>O4*O5+(O5-1)*O11+O7+O8</f>
         <v>1100</v>
       </c>
-      <c r="M22" s="14"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="17"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="Q3:Q6"/>
+  <mergeCells count="18">
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="C21:D22"/>
     <mergeCell ref="B2:E2"/>
@@ -1604,10 +1654,6 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G3:G4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O21:O22">
@@ -1633,23 +1679,293 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B2" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="G2" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B3" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="31">
+        <v>0.06</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="31">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B4" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="31">
+        <v>6</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B5" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="31">
+        <v>20</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="31">
+        <f>COUNTA(G13:G33)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B7" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="G7" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="28"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B8" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="G8" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B9" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="G9" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B11" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="28"/>
+      <c r="G11" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="32"/>
+      <c r="I11" s="28"/>
+      <c r="K11" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="L11" s="28"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B12" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="34">
+        <v>500</v>
+      </c>
+      <c r="E12" s="31">
+        <f>D12/1000</f>
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" s="34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B13" s="35"/>
+      <c r="C13" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="34">
+        <v>600</v>
+      </c>
+      <c r="E13" s="31">
+        <f t="shared" ref="E13:E15" si="0">D13/1000</f>
+        <v>0.6</v>
+      </c>
+      <c r="G13" s="29">
+        <v>1</v>
+      </c>
+      <c r="H13" s="29">
+        <v>1</v>
+      </c>
+      <c r="I13" s="29">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B14" s="35"/>
+      <c r="C14" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="34">
+        <v>700</v>
+      </c>
+      <c r="E14" s="31">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="G14" s="29">
+        <v>2</v>
+      </c>
+      <c r="H14" s="29">
+        <v>2</v>
+      </c>
+      <c r="I14" s="29">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B15" s="36"/>
+      <c r="C15" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="34">
+        <v>8000</v>
+      </c>
+      <c r="E15" s="31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G15" s="29">
+        <v>3</v>
+      </c>
+      <c r="H15" s="29">
+        <v>2</v>
+      </c>
+      <c r="I15" s="29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="G16" s="29">
+        <v>4</v>
+      </c>
+      <c r="H16" s="29">
+        <v>3</v>
+      </c>
+      <c r="I16" s="29">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.15">
+      <c r="G17" s="29">
+        <v>5</v>
+      </c>
+      <c r="H17" s="29">
+        <v>4</v>
+      </c>
+      <c r="I17" s="29">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.15">
+      <c r="G18" s="29">
+        <v>6</v>
+      </c>
+      <c r="H18" s="29">
+        <v>5</v>
+      </c>
+      <c r="I18" s="29">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.15">
+      <c r="G19" s="29">
+        <v>7</v>
+      </c>
+      <c r="H19" s="29">
+        <v>6</v>
+      </c>
+      <c r="I19" s="29">
+        <v>4885.8999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:B15"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.15">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B2" s="18" t="s">
         <v>29</v>
       </c>
@@ -1677,7 +1993,7 @@
       <c r="N2" s="19"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B3" s="21" t="s">
         <v>2</v>
       </c>
@@ -1718,8 +2034,8 @@
         <v>428.04</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B4" s="23"/>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B4" s="22"/>
       <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +2045,7 @@
       <c r="E4" s="5">
         <v>120.96</v>
       </c>
-      <c r="G4" s="23"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +2056,7 @@
         <f>I4/1000</f>
         <v>127.01</v>
       </c>
-      <c r="L4" s="23"/>
+      <c r="L4" s="22"/>
       <c r="M4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1751,7 +2067,7 @@
         <v>535.19000000000005</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B5" s="21" t="s">
         <v>30</v>
       </c>
@@ -1790,8 +2106,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B6" s="23"/>
       <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
@@ -1827,8 +2143,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B7" s="23"/>
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1866,8 +2182,8 @@
         <v>11.87</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B8" s="22"/>
       <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1878,7 +2194,7 @@
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="G8" s="22"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="9" t="s">
         <v>6</v>
       </c>
@@ -1889,7 +2205,7 @@
         <f t="shared" si="1"/>
         <v>13.087999999999999</v>
       </c>
-      <c r="L8" s="22"/>
+      <c r="L8" s="23"/>
       <c r="M8" s="9" t="s">
         <v>6</v>
       </c>
@@ -1901,7 +2217,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
         <v>31</v>
       </c>
@@ -1915,7 +2231,7 @@
         <f t="shared" si="0"/>
         <v>2.9</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1926,7 +2242,7 @@
         <f t="shared" si="1"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="L9" s="22"/>
+      <c r="L9" s="23"/>
       <c r="M9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1938,7 +2254,7 @@
         <v>7.94</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B10" s="8" t="s">
         <v>37</v>
       </c>
@@ -1951,7 +2267,7 @@
       <c r="E10" s="7">
         <v>0</v>
       </c>
-      <c r="G10" s="23"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="9" t="s">
         <v>8</v>
       </c>
@@ -1962,7 +2278,7 @@
         <f t="shared" si="1"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="L10" s="23"/>
+      <c r="L10" s="22"/>
       <c r="M10" s="9" t="s">
         <v>8</v>
       </c>
@@ -1974,11 +2290,11 @@
         <v>7.94</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
@@ -2012,8 +2328,8 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="G12" s="23"/>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="G12" s="22"/>
       <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
@@ -2024,7 +2340,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L12" s="23"/>
+      <c r="L12" s="22"/>
       <c r="M12" s="9" t="s">
         <v>17</v>
       </c>
@@ -2036,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.15">
       <c r="G13" s="9" t="s">
         <v>18</v>
       </c>
@@ -2050,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.15">
       <c r="G14" s="10" t="s">
         <v>74</v>
       </c>
@@ -2064,16 +2380,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B21" s="3">
         <f>E3+E7+E8+E10</f>
         <v>69.64</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16" t="str">
+      <c r="D21" s="15"/>
+      <c r="E21" s="24" t="str">
         <f>IF(AND(J3=B21,J4=B22),"OK","BAD")</f>
         <v>OK</v>
       </c>
@@ -2081,11 +2397,11 @@
         <f>IF((J13=0),J3*J6+(J6-1)*J12+J9+J10,J4*J6+(J6-1)*J12+J9+J10)</f>
         <v>428.04000000000008</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="16" t="str">
+      <c r="I21" s="15"/>
+      <c r="J21" s="24" t="str">
         <f>IF(AND(O3=G21,O4=G22),"OK","BAD")</f>
         <v>OK</v>
       </c>
@@ -2093,40 +2409,46 @@
         <f>O3*O6+(O6-1)*O12++O9+O10</f>
         <v>1300.0000000000002</v>
       </c>
-      <c r="M21" s="12" t="s">
+      <c r="M21" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="13"/>
-      <c r="O21" s="16" t="str">
+      <c r="N21" s="15"/>
+      <c r="O21" s="24" t="str">
         <f>IF(AND(1300=L21,1100=L22),"OK","BAD")</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B22" s="3">
         <f>E4+E5+E6+E9</f>
         <v>127.00999999999999</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="17"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="25"/>
       <c r="G22" s="1">
         <f>IF((J13=0),J4*J5+(J5-1)*J11+J7+J8,J3*J5+(J5-1)*J11+J7+J8)</f>
         <v>535.18999999999994</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="25"/>
       <c r="L22" s="1">
         <f>O4*O5+(O5-1)*O11+O7+O8</f>
         <v>1100</v>
       </c>
-      <c r="M22" s="14"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="17"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="L3:L4"/>
     <mergeCell ref="O21:O22"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="G7:G10"/>
@@ -2139,12 +2461,6 @@
     <mergeCell ref="H21:I22"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="M21:N22"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="L3:L4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O21:O22">
@@ -2167,25 +2483,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:J14"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.15">
       <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
@@ -2193,7 +2509,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B2" s="18" t="s">
         <v>41</v>
       </c>
@@ -2213,8 +2529,8 @@
       <c r="N2" s="19"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B3" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -2226,7 +2542,7 @@
       <c r="E3" s="5">
         <v>286.74</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="11" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -2239,7 +2555,7 @@
         <f>B21</f>
         <v>291.74</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="11" t="s">
         <v>47</v>
       </c>
       <c r="M3" s="9" t="s">
@@ -2253,8 +2569,8 @@
         <v>583.48</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B4" s="11"/>
       <c r="C4" s="9" t="s">
         <v>49</v>
       </c>
@@ -2264,7 +2580,7 @@
       <c r="E4" s="5">
         <v>191.16</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="9" t="s">
         <v>49</v>
       </c>
@@ -2275,7 +2591,7 @@
         <f>B22</f>
         <v>200.06</v>
       </c>
-      <c r="L4" s="26"/>
+      <c r="L4" s="11"/>
       <c r="M4" s="9" t="s">
         <v>49</v>
       </c>
@@ -2287,8 +2603,8 @@
         <v>400.12</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B5" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2325,8 +2641,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B6" s="11"/>
       <c r="C6" s="9" t="s">
         <v>55</v>
       </c>
@@ -2361,8 +2677,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B7" s="11"/>
       <c r="C7" s="9" t="s">
         <v>58</v>
       </c>
@@ -2372,7 +2688,7 @@
       <c r="E7" s="5">
         <v>2.5</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="11" t="s">
         <v>59</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -2384,7 +2700,7 @@
       <c r="J7" s="5">
         <v>0</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="L7" s="11" t="s">
         <v>60</v>
       </c>
       <c r="M7" s="9" t="s">
@@ -2397,8 +2713,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B8" s="11"/>
       <c r="C8" s="9" t="s">
         <v>61</v>
       </c>
@@ -2408,7 +2724,7 @@
       <c r="E8" s="5">
         <v>2.5</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="9" t="s">
         <v>55</v>
       </c>
@@ -2418,7 +2734,7 @@
       <c r="J8" s="5">
         <v>0</v>
       </c>
-      <c r="L8" s="26"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="9" t="s">
         <v>55</v>
       </c>
@@ -2429,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
         <v>62</v>
       </c>
@@ -2442,7 +2758,7 @@
       <c r="E9" s="5">
         <v>4</v>
       </c>
-      <c r="G9" s="26"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="9" t="s">
         <v>58</v>
       </c>
@@ -2452,7 +2768,7 @@
       <c r="J9" s="5">
         <v>0</v>
       </c>
-      <c r="L9" s="26"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="9" t="s">
         <v>58</v>
       </c>
@@ -2463,7 +2779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B10" s="8" t="s">
         <v>64</v>
       </c>
@@ -2476,7 +2792,7 @@
       <c r="E10" s="7">
         <v>0</v>
       </c>
-      <c r="G10" s="26"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="9" t="s">
         <v>61</v>
       </c>
@@ -2486,7 +2802,7 @@
       <c r="J10" s="5">
         <v>0</v>
       </c>
-      <c r="L10" s="26"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="9" t="s">
         <v>61</v>
       </c>
@@ -2497,18 +2813,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B11" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="11" t="s">
         <v>68</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -2521,7 +2837,7 @@
         <f t="shared" ref="J11:J12" si="0">I11/1000</f>
         <v>0</v>
       </c>
-      <c r="L11" s="26" t="s">
+      <c r="L11" s="11" t="s">
         <v>70</v>
       </c>
       <c r="M11" s="9" t="s">
@@ -2534,8 +2850,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="G12" s="26"/>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="G12" s="11"/>
       <c r="H12" s="9" t="s">
         <v>71</v>
       </c>
@@ -2546,7 +2862,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L12" s="26"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="9" t="s">
         <v>71</v>
       </c>
@@ -2557,7 +2873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.15">
       <c r="G13" s="9" t="s">
         <v>72</v>
       </c>
@@ -2571,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.15">
       <c r="G14" s="9" t="s">
         <v>74</v>
       </c>
@@ -2585,16 +2901,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B21" s="3">
         <f>E3+E7+E8+E10</f>
         <v>291.74</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16" t="str">
+      <c r="D21" s="15"/>
+      <c r="E21" s="24" t="str">
         <f>IF(AND(J3=B21,J4=B22),"OK","BAD")</f>
         <v>OK</v>
       </c>
@@ -2602,11 +2918,11 @@
         <f>IF((J13=0),J3*J6+(J6-1)*J12+J9+J10,J4*J6+(J6-1)*J12+J9+J10)</f>
         <v>583.48</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="16" t="str">
+      <c r="I21" s="15"/>
+      <c r="J21" s="24" t="str">
         <f>IF(AND(O3=G21,O4=G22),"OK","BAD")</f>
         <v>OK</v>
       </c>
@@ -2614,40 +2930,46 @@
         <f>O3*O6+(O6-1)*O12++O9+O10</f>
         <v>1171.96</v>
       </c>
-      <c r="M21" s="12" t="s">
+      <c r="M21" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="N21" s="13"/>
-      <c r="O21" s="16" t="str">
+      <c r="N21" s="15"/>
+      <c r="O21" s="24" t="str">
         <f>IF(AND(1300=L21,1100=L22),"OK","BAD")</f>
         <v>BAD</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B22" s="3">
         <f>E4+E5+E6+E9</f>
         <v>200.06</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="17"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="25"/>
       <c r="G22" s="1">
         <f>IF((J13=0),J4*J5+(J5-1)*J11+J7+J8,J3*J5+(J5-1)*J11+J7+J8)</f>
         <v>400.12</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="25"/>
       <c r="L22" s="1">
         <f>O4*O5+(O5-1)*O11+O7+O8</f>
         <v>1210.3600000000001</v>
       </c>
-      <c r="M22" s="14"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="17"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="L3:L4"/>
     <mergeCell ref="O21:O22"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="G7:G10"/>
@@ -2660,12 +2982,6 @@
     <mergeCell ref="H21:I22"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="M21:N22"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="L3:L4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O21:O22">

</xml_diff>